<commit_message>
update ACMG of go
</commit_message>
<xml_diff>
--- a/template/Tier3.xlsx
+++ b/template/Tier3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangyaoshen\go\src\github.com\liserjrqlxue\anno2xlsx\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DC6AF2-5300-4382-81E1-FFC5E0478F29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BF799A-85CB-4EE9-A300-DCF10ECA00FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2790" yWindow="0" windowWidth="28800" windowHeight="11175" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="总表" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">总表!$F$1:$Y$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">总表!$A$1:$AD$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>SampleID</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>自动化判断</t>
-  </si>
-  <si>
-    <t>变异来源</t>
   </si>
   <si>
     <t>GnomAD AF</t>
@@ -99,6 +96,30 @@
   </si>
   <si>
     <t>Call</t>
+  </si>
+  <si>
+    <t>Tier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MutationNameLite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>变异来源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExAC AF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MatEntScan pred</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>引物设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -156,13 +177,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -502,32 +525,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCAAEFA0-5F78-49F1-9E1F-85C060BBE36D}">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AA1:AD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="5" width="8.796875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.796875" hidden="1" customWidth="1"/>
+    <col min="27" max="30" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -541,57 +567,72 @@
       <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>18</v>
+      <c r="Z1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:Y1" xr:uid="{6B971EAE-5AFB-4437-A7F0-CF152F9344F6}"/>
+  <autoFilter ref="A1:AD1" xr:uid="{27691CEA-5939-4AB2-988B-78CD0C6C1FEB}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>